<commit_message>
automation + lifetimes batch8 442
</commit_message>
<xml_diff>
--- a/Batch 8/Red Bulk.xlsx
+++ b/Batch 8/Red Bulk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftamb\Documents\GitHub\Palsfit\Batch 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE11CB57-CCF1-4F10-9B18-06E4829A97AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FADF9A0-309B-4E66-9433-EEB61CC44606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B1D783F5-17AA-4934-97D6-37ACE32566A0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Bulk Lifetime</t>
   </si>
@@ -86,6 +86,45 @@
   <si>
     <t>I2 (Kanda)</t>
   </si>
+  <si>
+    <t>80-20</t>
+  </si>
+  <si>
+    <t>70-30</t>
+  </si>
+  <si>
+    <t>50-50</t>
+  </si>
+  <si>
+    <t>40-60</t>
+  </si>
+  <si>
+    <t>30-70</t>
+  </si>
+  <si>
+    <t>10-90</t>
+  </si>
+  <si>
+    <t>5-95</t>
+  </si>
+  <si>
+    <t>R.Bulk</t>
+  </si>
+  <si>
+    <t>tau_3</t>
+  </si>
+  <si>
+    <t>rel I2</t>
+  </si>
+  <si>
+    <t>rel I1</t>
+  </si>
+  <si>
+    <t>abs I1</t>
+  </si>
+  <si>
+    <t>abs I2</t>
+  </si>
 </sst>
 </file>
 
@@ -94,8 +133,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,11 +170,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3681,10 +3730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155A6553-7559-4F22-B39F-ECD130D26314}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="J32" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4368,9 +4417,212 @@
         <v>1E+18</v>
       </c>
     </row>
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="2">
+        <f>H2</f>
+        <v>0.80465558145450566</v>
+      </c>
+      <c r="J35" s="2">
+        <f>1-I35</f>
+        <v>0.19534441854549434</v>
+      </c>
+      <c r="K35" s="3">
+        <f>G2</f>
+        <v>332.24219377854445</v>
+      </c>
+      <c r="L35" s="2">
+        <f>(100%-$I$43)*I35</f>
+        <v>0.80344859808232394</v>
+      </c>
+      <c r="M35" s="2">
+        <f>(100%-$I$43)*J35</f>
+        <v>0.19505140191767611</v>
+      </c>
+    </row>
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2">
+        <f>H3</f>
+        <v>0.67315793588062067</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" ref="J36:J41" si="8">1-I36</f>
+        <v>0.32684206411937933</v>
+      </c>
+      <c r="K36" s="3">
+        <f>G3</f>
+        <v>325.74854902563709</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" ref="L36:L41" si="9">(100%-$I$43)*I36</f>
+        <v>0.67214819897679978</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" ref="M36:M41" si="10">(100%-$I$43)*J36</f>
+        <v>0.32635180102320027</v>
+      </c>
+    </row>
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="2">
+        <f>H4</f>
+        <v>0.50733840453527779</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="8"/>
+        <v>0.49266159546472221</v>
+      </c>
+      <c r="K37" s="3">
+        <f>G4</f>
+        <v>313.49411851742252</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="9"/>
+        <v>0.50657739692847492</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="10"/>
+        <v>0.49192260307152513</v>
+      </c>
+    </row>
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="2">
+        <f>H5</f>
+        <v>0.40706560847116635</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="8"/>
+        <v>0.59293439152883365</v>
+      </c>
+      <c r="K38" s="3">
+        <f>G5</f>
+        <v>302.12826637196537</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="9"/>
+        <v>0.40645501005845963</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="10"/>
+        <v>0.59204498994154042</v>
+      </c>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="2">
+        <f>H7</f>
+        <v>0.291742739370212</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="8"/>
+        <v>0.708257260629788</v>
+      </c>
+      <c r="K39" s="3">
+        <f>G7</f>
+        <v>281.7018447731428</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="9"/>
+        <v>0.29130512526115671</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="10"/>
+        <v>0.70719487473884335</v>
+      </c>
+    </row>
+    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="2">
+        <f>H9</f>
+        <v>9.3364494988434799E-2</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.9066355050115652</v>
+      </c>
+      <c r="K40" s="3">
+        <f>G9</f>
+        <v>186.9210410233789</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="9"/>
+        <v>9.3224448245952149E-2</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="10"/>
+        <v>0.90527555175404795</v>
+      </c>
+    </row>
+    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="2">
+        <f>H11</f>
+        <v>4.8968192789354603E-2</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="8"/>
+        <v>0.9510318072106454</v>
+      </c>
+      <c r="K41" s="3">
+        <f>G11</f>
+        <v>129.0347137637028</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="9"/>
+        <v>4.8894740500170571E-2</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="10"/>
+        <v>0.94960525949982943</v>
+      </c>
+    </row>
+    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43" s="2">
+        <v>1.5E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="H40" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>